<commit_message>
alterações no PB e no BPMN
</commit_message>
<xml_diff>
--- a/Documentação/PRODUCT BACKLOG - SPORT.FY.xlsx
+++ b/Documentação/PRODUCT BACKLOG - SPORT.FY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/alex_barreira_bandtec_com_br/Documents/ALEX -BANTEC/0 - ACADÊMICO/2. GRADUAÇÃO BANDTEC GF/2021 1/ANALISE DE SISTEMAS/Aulas/Aula 03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz.sousa\Documents\GitHub\grupo3-provisorio\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E353FDFA-C6D4-4973-8E9F-74C240CC0C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E70479-D3A8-4CA2-A558-BB04B1CAB1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
     <t>Product BackLog Classified (PBC)</t>
   </si>
@@ -215,15 +215,6 @@
     <t>US#12.1&lt;Esporte&gt;</t>
   </si>
   <si>
-    <t>O sistema tera a opção de volei</t>
-  </si>
-  <si>
-    <t>US#12.2&lt;Esporte&gt;</t>
-  </si>
-  <si>
-    <t>O sistema tera a opção de tenis</t>
-  </si>
-  <si>
     <t>JU#14&lt;&gt;</t>
   </si>
   <si>
@@ -357,6 +348,21 @@
   </si>
   <si>
     <t>EC</t>
+  </si>
+  <si>
+    <t>O sistema tera a opção de basquete</t>
+  </si>
+  <si>
+    <t>US#12&lt;Avalição&gt;</t>
+  </si>
+  <si>
+    <t>O sistema fornece avaliação entre times</t>
+  </si>
+  <si>
+    <t>O sistema fornece cadastro de times</t>
+  </si>
+  <si>
+    <t>o sistema tera mais que um plano</t>
   </si>
 </sst>
 </file>
@@ -786,27 +792,27 @@
     </xf>
   </cellXfs>
   <cellStyles count="22">
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="21" builtinId="8"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
@@ -1682,23 +1688,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="23.15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="11" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" style="14" customWidth="1"/>
-    <col min="4" max="4" width="78.85546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="0.7109375" style="15" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="13" customWidth="1"/>
-    <col min="9" max="10" width="8.85546875" style="13"/>
-    <col min="11" max="11" width="13.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="13"/>
+    <col min="3" max="3" width="42.7265625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="78.81640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="0.7265625" style="15" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" style="13" customWidth="1"/>
+    <col min="9" max="10" width="8.81640625" style="13"/>
+    <col min="11" max="11" width="13.7265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="19.5" customHeight="1" thickBot="1"/>
@@ -1713,8 +1719,8 @@
       <c r="G2" s="41"/>
       <c r="H2" s="42"/>
     </row>
-    <row r="3" spans="2:8" ht="9.9499999999999993" customHeight="1" thickBot="1"/>
-    <row r="4" spans="2:8" s="22" customFormat="1" ht="24.95" customHeight="1" thickBot="1">
+    <row r="3" spans="2:8" ht="10" customHeight="1" thickBot="1"/>
+    <row r="4" spans="2:8" s="22" customFormat="1" ht="25" customHeight="1" thickBot="1">
       <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
@@ -1737,7 +1743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="5" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B5" s="23" t="s">
         <v>8</v>
       </c>
@@ -1754,7 +1760,7 @@
       </c>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="6" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B6" s="23" t="s">
         <v>8</v>
       </c>
@@ -1771,7 +1777,7 @@
       </c>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="7" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
@@ -1788,7 +1794,7 @@
       </c>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="8" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B8" s="23" t="s">
         <v>8</v>
       </c>
@@ -1822,7 +1828,7 @@
       </c>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="10" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
@@ -1839,7 +1845,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="11" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B11" s="23" t="s">
         <v>8</v>
       </c>
@@ -1856,7 +1862,7 @@
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="12" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B12" s="23" t="s">
         <v>8</v>
       </c>
@@ -1873,7 +1879,7 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="13" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B13" s="23" t="s">
         <v>8</v>
       </c>
@@ -1890,7 +1896,7 @@
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="14" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="B14" s="23" t="s">
         <v>8</v>
       </c>
@@ -1907,7 +1913,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:8" s="27" customFormat="1" ht="15">
+    <row r="15" spans="2:8" s="27" customFormat="1" ht="14.5">
       <c r="B15" s="23" t="s">
         <v>8</v>
       </c>
@@ -1924,7 +1930,7 @@
       <c r="G15" s="31"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="2:8" s="27" customFormat="1" ht="30">
+    <row r="16" spans="2:8" s="27" customFormat="1" ht="29">
       <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
@@ -1941,7 +1947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="17" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B17" s="23" t="s">
         <v>8</v>
       </c>
@@ -1958,7 +1964,7 @@
       </c>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="18" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B18" s="23" t="s">
         <v>8</v>
       </c>
@@ -1975,7 +1981,7 @@
       </c>
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="19" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B19" s="23" t="s">
         <v>8</v>
       </c>
@@ -1983,7 +1989,7 @@
         <v>39</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="26"/>
@@ -1992,55 +1998,59 @@
       </c>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="20" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B20" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="E20" s="30"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26" t="s">
+      <c r="F20" s="26" t="s">
         <v>11</v>
       </c>
+      <c r="G20" s="26"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="21" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B21" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="29"/>
+        <v>40</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>88</v>
+      </c>
       <c r="E21" s="30"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="22" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B22" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="29"/>
+        <v>41</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>89</v>
+      </c>
       <c r="E22" s="30"/>
       <c r="F22" s="26"/>
       <c r="G22" s="26"/>
       <c r="H22" s="26"/>
     </row>
-    <row r="23" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="23" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B23" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="30"/>
@@ -2048,12 +2058,12 @@
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
     </row>
-    <row r="24" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="24" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B24" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
@@ -2061,7 +2071,7 @@
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
     </row>
-    <row r="25" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="25" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B25" s="23" t="s">
         <v>8</v>
       </c>
@@ -2072,7 +2082,7 @@
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
     </row>
-    <row r="26" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="26" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B26" s="23" t="s">
         <v>8</v>
       </c>
@@ -2083,7 +2093,7 @@
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="27" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B27" s="23" t="s">
         <v>8</v>
       </c>
@@ -2094,7 +2104,7 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="28" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B28" s="23" t="s">
         <v>8</v>
       </c>
@@ -2105,7 +2115,7 @@
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="29" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B29" s="23" t="s">
         <v>8</v>
       </c>
@@ -2116,7 +2126,7 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="30" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B30" s="23" t="s">
         <v>8</v>
       </c>
@@ -2127,7 +2137,7 @@
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
     </row>
-    <row r="31" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="31" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B31" s="23" t="s">
         <v>8</v>
       </c>
@@ -2138,7 +2148,7 @@
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="32" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B32" s="23" t="s">
         <v>8</v>
       </c>
@@ -2149,7 +2159,7 @@
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
     </row>
-    <row r="33" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="33" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B33" s="23" t="s">
         <v>8</v>
       </c>
@@ -2160,7 +2170,7 @@
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
     </row>
-    <row r="34" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="34" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B34" s="23" t="s">
         <v>8</v>
       </c>
@@ -2171,87 +2181,87 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
     </row>
-    <row r="35" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="35" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C35" s="33"/>
       <c r="E35" s="34"/>
       <c r="G35" s="35"/>
     </row>
-    <row r="36" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="36" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C36" s="33"/>
       <c r="E36" s="34"/>
       <c r="G36" s="35"/>
     </row>
-    <row r="37" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="37" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C37" s="33"/>
       <c r="E37" s="34"/>
       <c r="G37" s="35"/>
     </row>
-    <row r="38" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="38" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C38" s="33"/>
       <c r="E38" s="34"/>
       <c r="G38" s="35"/>
     </row>
-    <row r="39" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="39" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C39" s="33"/>
       <c r="E39" s="34"/>
       <c r="G39" s="35"/>
     </row>
-    <row r="40" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="40" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C40" s="33"/>
       <c r="E40" s="34"/>
       <c r="G40" s="35"/>
     </row>
-    <row r="41" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="41" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C41" s="33"/>
       <c r="E41" s="34"/>
       <c r="G41" s="35"/>
     </row>
-    <row r="42" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="42" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C42" s="33"/>
       <c r="E42" s="34"/>
       <c r="G42" s="35"/>
     </row>
-    <row r="43" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="43" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C43" s="33"/>
       <c r="E43" s="34"/>
       <c r="G43" s="35"/>
     </row>
-    <row r="44" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="44" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C44" s="33"/>
       <c r="E44" s="34"/>
       <c r="G44" s="35"/>
     </row>
-    <row r="45" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="45" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C45" s="33"/>
       <c r="E45" s="34"/>
       <c r="G45" s="35"/>
     </row>
-    <row r="46" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="46" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C46" s="33"/>
       <c r="E46" s="34"/>
       <c r="G46" s="35"/>
     </row>
-    <row r="47" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="47" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C47" s="33"/>
       <c r="E47" s="34"/>
       <c r="G47" s="35"/>
     </row>
-    <row r="48" spans="2:8" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="48" spans="2:8" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C48" s="33"/>
       <c r="E48" s="34"/>
       <c r="G48" s="35"/>
     </row>
-    <row r="49" spans="3:7" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="49" spans="3:7" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C49" s="33"/>
       <c r="E49" s="34"/>
       <c r="G49" s="35"/>
     </row>
-    <row r="50" spans="3:7" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="50" spans="3:7" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C50" s="33"/>
       <c r="E50" s="34"/>
       <c r="G50" s="35"/>
     </row>
-    <row r="51" spans="3:7" s="27" customFormat="1" ht="23.1" customHeight="1">
+    <row r="51" spans="3:7" s="27" customFormat="1" ht="23.15" customHeight="1">
       <c r="C51" s="33"/>
       <c r="E51" s="34"/>
       <c r="G51" s="35"/>
@@ -2370,52 +2380,52 @@
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="52.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="52.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2423,34 +2433,34 @@
         <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="7"/>
       <c r="B7" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="7"/>
       <c r="B9" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2467,105 +2477,105 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
     </row>
     <row r="16" spans="1:8" ht="68.25" customHeight="1">
       <c r="A16" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23.5">
+      <c r="A17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="12" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="23.5">
+      <c r="A18" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="23.25">
-      <c r="A17" s="10" t="s">
+      <c r="B18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="6" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="23.5">
+      <c r="A19" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.25">
-      <c r="A18" s="10" t="s">
+      <c r="B19" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="6" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="23.5">
+      <c r="A20" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="23.25">
-      <c r="A19" s="10" t="s">
+      <c r="B20" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="6" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="23.5">
+      <c r="A21" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="23.25">
-      <c r="A20" s="10" t="s">
+      <c r="B21" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="6" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="23.5">
+      <c r="A22" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="23.25">
-      <c r="A21" s="10" t="s">
+      <c r="B22" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="6" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="23.5">
+      <c r="A23" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="23.25">
-      <c r="A22" s="10" t="s">
+      <c r="B23" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="6" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="23.5">
+      <c r="A24" s="10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="23.25">
-      <c r="A23" s="10" t="s">
+      <c r="B24" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="6" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="23.5">
+      <c r="A25" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="23.25">
-      <c r="A24" s="10" t="s">
+      <c r="B25" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="6" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="23.5">
+      <c r="A26" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="23.25">
-      <c r="A25" s="10" t="s">
+      <c r="B26" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="6" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="23.5">
+      <c r="A27" s="10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="23.25">
-      <c r="A26" s="10" t="s">
+      <c r="B27" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="23.25">
-      <c r="A27" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2583,7 +2593,7 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>